<commit_message>
dev: fix wrong spell; add Action fileds
</commit_message>
<xml_diff>
--- a/test/data/test-mbus-devices-sheet1.xlsx
+++ b/test/data/test-mbus-devices-sheet1.xlsx
@@ -47,7 +47,7 @@
     <t>Frequency</t>
   </si>
   <si>
-    <t>FataLength</t>
+    <t>DataLength</t>
   </si>
   <si>
     <t>Weight</t>
@@ -240,7 +240,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -250,18 +250,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -605,7 +593,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -629,16 +617,16 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -647,89 +635,89 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -737,12 +725,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1273,7 +1255,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="7"/>
@@ -1308,85 +1290,85 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>100</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="2">
         <v>4</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>100</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <v>4</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>100</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <v>4</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="2">
         <v>1</v>
       </c>
     </row>

</xml_diff>